<commit_message>
project euler first 4
</commit_message>
<xml_diff>
--- a/100 programming challenges.xlsx
+++ b/100 programming challenges.xlsx
@@ -390,12 +390,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -405,11 +420,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="İyi" xfId="1" builtinId="26"/>
@@ -696,7 +712,7 @@
   <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A101" sqref="A1:A101"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,27 +746,27 @@
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -760,7 +776,7 @@
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -790,7 +806,7 @@
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -820,7 +836,7 @@
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>